<commit_message>
Changes required for Grand Report security checks are made.
</commit_message>
<xml_diff>
--- a/atp-dataset-import/TEST_DATA/importVariablesWithMacros_1.xlsx
+++ b/atp-dataset-import/TEST_DATA/importVariablesWithMacros_1.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ATP\dataset\atp-dataset\netcracker-atp-dataset-import\TEST_DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\qstp_projects\qubership-testing-platform-datasets\atp-dataset-import\TEST_DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="DJR_6620" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -42,9 +42,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>$EXECUTION_REQUEST_NUMBER()at@yandex.ru</t>
-  </si>
-  <si>
     <t>Rest</t>
   </si>
   <si>
@@ -88,12 +85,15 @@
   </si>
   <si>
     <t>AT$ENV_VARIABLE(LOGIN_TENANT)</t>
+  </si>
+  <si>
+    <t>$EXECUTION_REQUEST_NUMBER()example@example.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -163,18 +163,18 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -387,9 +387,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -427,7 +427,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -499,7 +499,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -652,199 +652,204 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="43.140625" customWidth="1"/>
+    <col min="4" max="4" width="43.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="6"/>
+      <c r="D15" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
@@ -855,11 +860,6 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.5" footer="0.5"/>
   <pageSetup pageOrder="overThenDown" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>